<commit_message>
More changes to frontend
</commit_message>
<xml_diff>
--- a/Screener/Financial Values.xlsx
+++ b/Screener/Financial Values.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
   <si>
     <t>Objective</t>
   </si>
@@ -101,12 +101,6 @@
     <t>debttoequity</t>
   </si>
   <si>
-    <t>Order</t>
-  </si>
-  <si>
-    <t>asc</t>
-  </si>
-  <si>
     <t>View</t>
   </si>
   <si>
@@ -128,13 +122,10 @@
     <t>pricetorevenue</t>
   </si>
   <si>
-    <t>desc</t>
-  </si>
-  <si>
     <t>Free Cash Flow to Firm</t>
   </si>
   <si>
-    <t>freecashflow</t>
+    <t>fcffgrowth</t>
   </si>
 </sst>
 </file>
@@ -452,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,10 +600,10 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
         <v>23</v>
@@ -623,44 +614,44 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -683,38 +674,24 @@
         <v>2000000000</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B12" t="s">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" t="s">
-        <v>34</v>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12">
+        <v>-99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>